<commit_message>
Antes de ordenar las imagenes
</commit_message>
<xml_diff>
--- a/Ideas/planilla de paguianas.xlsx
+++ b/Ideas/planilla de paguianas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>index</t>
   </si>
@@ -246,16 +246,43 @@
     <t>ID-imagen</t>
   </si>
   <si>
-    <t>galeria</t>
-  </si>
-  <si>
-    <t>ID-comentario</t>
-  </si>
-  <si>
-    <t>ID-imagen(f)</t>
-  </si>
-  <si>
-    <t>tags ves como lopongo</t>
+    <t>ID-galeria</t>
+  </si>
+  <si>
+    <t>dibujos</t>
+  </si>
+  <si>
+    <t>ID-usuario</t>
+  </si>
+  <si>
+    <t>ID-box-tags</t>
+  </si>
+  <si>
+    <t>ID-tags</t>
+  </si>
+  <si>
+    <t>nombre-tag</t>
+  </si>
+  <si>
+    <t>dibujo</t>
+  </si>
+  <si>
+    <t>arte conceptual</t>
+  </si>
+  <si>
+    <t>renacentista</t>
+  </si>
+  <si>
+    <t>diseño de entorno</t>
+  </si>
+  <si>
+    <t>videojuegos</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>ID-box-tags-imagen</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1099,8 +1126,6 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
@@ -1427,9 +1452,18 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="C20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="A20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
@@ -1630,18 +1664,28 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="D32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="A32" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="G33" s="2"/>
+      <c r="J33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -1649,28 +1693,90 @@
         <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="G36" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2">
+        <v>2</v>
+      </c>
+      <c r="K36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="J37" s="2">
+        <v>3</v>
+      </c>
+      <c r="K37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="J38" s="2">
+        <v>4</v>
+      </c>
+      <c r="K38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="J39" s="2">
+        <v>5</v>
+      </c>
+      <c r="K39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A32:I32"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>

</xml_diff>